<commit_message>
feat: 排除小於 1:100 的 denom
</commit_message>
<xml_diff>
--- a/input/currency_exchange_rate.xlsx
+++ b/input/currency_exchange_rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\chiisen\coin_size\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D42AB8-264E-42B5-B521-EB69E0825EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91777E64-59FF-40FA-9224-8FF3962EEEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29370" yWindow="450" windowWidth="26055" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="435" yWindow="675" windowWidth="26055" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="currency_exchange_rate" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="133">
   <si>
     <t>ExCurrency</t>
   </si>
@@ -36,28 +36,394 @@
     <t>EnableTime</t>
   </si>
   <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t>2022-07-07 04:00:00</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>2022-07-13 04:00:00</t>
+  </si>
+  <si>
+    <t>ARS</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>AUD2</t>
+  </si>
+  <si>
+    <t>AZN</t>
+  </si>
+  <si>
+    <t>BDT</t>
+  </si>
+  <si>
+    <t>BGN</t>
+  </si>
+  <si>
+    <t>BMD</t>
+  </si>
+  <si>
+    <t>2020-03-23 00:56:28</t>
+  </si>
+  <si>
+    <t>BND</t>
+  </si>
+  <si>
+    <t>2022-03-04 15:00:00</t>
+  </si>
+  <si>
+    <t>BOB</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>BZD</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>CAD2</t>
+  </si>
+  <si>
+    <t>CHF</t>
+  </si>
+  <si>
+    <t>CHF2</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>CNY</t>
+  </si>
+  <si>
+    <t>2015-08-10 10:15:04</t>
+  </si>
+  <si>
+    <t>CNY2</t>
+  </si>
+  <si>
+    <t>2021-11-29 03:00:00</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>DKK</t>
+  </si>
+  <si>
+    <t>DOG</t>
+  </si>
+  <si>
+    <t>DOP</t>
+  </si>
+  <si>
+    <t>DZD</t>
+  </si>
+  <si>
+    <t>ETB</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>EUR2</t>
+  </si>
+  <si>
+    <t>FIM</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>GBP2</t>
+  </si>
+  <si>
+    <t>GEL</t>
+  </si>
+  <si>
+    <t>GHS</t>
+  </si>
+  <si>
+    <t>HKD</t>
+  </si>
+  <si>
+    <t>HKD2</t>
+  </si>
+  <si>
+    <t>HNL</t>
+  </si>
+  <si>
+    <t>HRK</t>
+  </si>
+  <si>
+    <t>HUF</t>
+  </si>
+  <si>
+    <t>IDR</t>
+  </si>
+  <si>
+    <t>IDR2</t>
+  </si>
+  <si>
+    <t>IDS</t>
+  </si>
+  <si>
+    <t>2020-03-23 01:26:56</t>
+  </si>
+  <si>
+    <t>ILS</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>INR2</t>
+  </si>
+  <si>
+    <t>IRR</t>
+  </si>
+  <si>
+    <t>ISK</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>JPY2</t>
+  </si>
+  <si>
     <t>KBB</t>
   </si>
   <si>
     <t>2022-01-24 00:00:00</t>
   </si>
   <si>
-    <t>BMD</t>
+    <t>KES</t>
+  </si>
+  <si>
+    <t>KGS</t>
+  </si>
+  <si>
+    <t>KHR</t>
+  </si>
+  <si>
+    <t>KRW</t>
+  </si>
+  <si>
+    <t>KRW2</t>
+  </si>
+  <si>
+    <t>KZT</t>
+  </si>
+  <si>
+    <t>LAK</t>
+  </si>
+  <si>
+    <t>LKR</t>
+  </si>
+  <si>
+    <t>LRD</t>
+  </si>
+  <si>
+    <t>MAD</t>
+  </si>
+  <si>
+    <t>MDL</t>
+  </si>
+  <si>
+    <t>MMK</t>
+  </si>
+  <si>
+    <t>MMK2</t>
+  </si>
+  <si>
+    <t>MNT</t>
+  </si>
+  <si>
+    <t>MOP</t>
+  </si>
+  <si>
+    <t>MXN</t>
+  </si>
+  <si>
+    <t>MYR</t>
+  </si>
+  <si>
+    <t>MYR2</t>
+  </si>
+  <si>
+    <t>NGN</t>
+  </si>
+  <si>
+    <t>NIO</t>
+  </si>
+  <si>
+    <t>NLG</t>
+  </si>
+  <si>
+    <t>2021-02-03 00:00:00</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>NOK2</t>
+  </si>
+  <si>
+    <t>NPR</t>
+  </si>
+  <si>
+    <t>NTD</t>
+  </si>
+  <si>
+    <t>2022-05-12 03:00:00</t>
+  </si>
+  <si>
+    <t>NZD</t>
+  </si>
+  <si>
+    <t>NZD2</t>
+  </si>
+  <si>
+    <t>PEN</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>PHP2</t>
+  </si>
+  <si>
+    <t>PLN</t>
+  </si>
+  <si>
+    <t>PYG</t>
+  </si>
+  <si>
+    <t>RON</t>
+  </si>
+  <si>
+    <t>2022-07-07 05:00:00</t>
+  </si>
+  <si>
+    <t>RSD</t>
+  </si>
+  <si>
+    <t>RUB</t>
+  </si>
+  <si>
+    <t>RUP</t>
+  </si>
+  <si>
+    <t>SAR</t>
+  </si>
+  <si>
+    <t>SEK</t>
+  </si>
+  <si>
+    <t>SEK2</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>2022-07-07 06:00:00</t>
+  </si>
+  <si>
+    <t>SGD2</t>
+  </si>
+  <si>
+    <t>SLE</t>
+  </si>
+  <si>
+    <t>2022-09-22 01:00:00</t>
+  </si>
+  <si>
+    <t>SLL</t>
+  </si>
+  <si>
+    <t>THB</t>
+  </si>
+  <si>
+    <t>THB2</t>
+  </si>
+  <si>
+    <t>TND</t>
+  </si>
+  <si>
+    <t>TRY</t>
+  </si>
+  <si>
+    <t>TWD</t>
+  </si>
+  <si>
+    <t>TZS</t>
+  </si>
+  <si>
+    <t>UAH</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>USD2</t>
+  </si>
+  <si>
+    <t>USDT</t>
+  </si>
+  <si>
+    <t>UYU</t>
+  </si>
+  <si>
+    <t>VDO</t>
+  </si>
+  <si>
+    <t>VEF</t>
+  </si>
+  <si>
+    <t>VES</t>
   </si>
   <si>
     <t>VND</t>
   </si>
   <si>
-    <t>2022-07-07 06:00:00</t>
-  </si>
-  <si>
-    <t>GBP</t>
-  </si>
-  <si>
-    <t>2022-07-07 04:00:00</t>
-  </si>
-  <si>
-    <t>2020-03-23 00:56:28</t>
+    <t>VND2</t>
+  </si>
+  <si>
+    <t>VNS</t>
+  </si>
+  <si>
+    <t>XAF</t>
+  </si>
+  <si>
+    <t>XOF</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>ZAR</t>
+  </si>
+  <si>
+    <t>ZAR2</t>
+  </si>
+  <si>
+    <t>ZMW</t>
   </si>
 </sst>
 </file>
@@ -422,11 +788,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -447,48 +813,1291 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0.54857299999999998</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>0.14113000000000001</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B3">
-        <v>0.12310400000000001</v>
+        <v>62.7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>573.86215800000002</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.216665</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2.1599999999999999E-4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.25378899999999999</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>13.932520999999999</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0.27945700000000001</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>0.14113000000000001</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>0.212894</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>1.02</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0.77401699999999996</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>0.3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>0.19243099999999999</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>1.92E-4</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>0.142487</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>1.4200000000000001E-4</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>131.99</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>1E-3</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>582.45000000000005</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>103.24766</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>3.5347789999999999</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>1.05</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>1.223579</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>8.18</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>21.82</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>7.78</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>0.14290700000000001</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <v>1.4200000000000001E-4</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32">
+        <v>0.84969099999999997</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>0.12310400000000001</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>1.2300000000000001E-4</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>0.43905699999999998</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>1.1976450000000001</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>1.172099</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>1.1720000000000001E-3</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39">
+        <v>3.6824210000000002</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40">
+        <v>1.075947</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41">
+        <v>56.294342</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42">
+        <v>2220.1876000000002</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43">
+        <v>2.2201870000000001</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44">
+        <v>2.3700700000000001</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45">
+        <v>0.51</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46">
+        <v>11.783842999999999</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47">
+        <v>1.1783E-2</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48">
+        <v>6301.21</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49">
+        <v>19.937564999999999</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50">
+        <v>20.408073999999999</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51">
+        <v>2.0407999999999999E-2</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52">
+        <v>573.86215800000002</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53">
+        <v>17.600272</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <v>11.876369</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55">
+        <v>607.46348999999998</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56">
+        <v>193.92475999999999</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57">
+        <v>0.19392400000000001</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58">
+        <v>69.938070999999994</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59">
+        <v>2243.6170999999999</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60">
+        <v>53.399526000000002</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61">
+        <v>22.67</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62">
+        <v>1.49</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63">
+        <v>2.8786309999999999</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64">
+        <v>278.50857999999999</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65">
+        <v>0.27850799999999998</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66">
+        <v>469.44308999999998</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67">
+        <v>1.2</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68">
+        <v>3</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69">
+        <v>0.65789299999999995</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70">
+        <v>6.5700000000000003E-4</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71">
+        <v>62.009388000000001</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B72">
+        <v>5.3725120000000004</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B73">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74">
+        <v>1.475468</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B75">
+        <v>1.475E-3</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B76">
+        <v>18.871894999999999</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B77">
+        <v>441.3</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78">
+        <v>0.240207</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80">
+        <v>0.56515599999999999</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81">
+        <v>8.1940380000000008</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82">
+        <v>8.1939999999999999E-3</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83">
+        <v>0.65</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84">
+        <v>1026.52</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85">
+        <v>0.70635000000000003</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B86">
+        <v>16.783677999999998</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B87">
+        <v>7.927378</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B88">
+        <v>42.857754999999997</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B89">
+        <v>0.56017700000000004</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B90">
+        <v>1.5276639999999999</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91">
+        <v>1.5269999999999999E-3</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B92">
+        <v>0.20786499999999999</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93">
+        <v>2.0699999999999999E-4</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B94">
+        <v>1.9559200000000001</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B95">
+        <v>1955.92</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B96">
+        <v>5.2745980000000001</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B97">
+        <v>5.274E-3</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B98">
+        <v>0.46002300000000002</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B99">
+        <v>2.4861550000000001</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B100">
+        <v>4.446885</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B101">
+        <v>348.40429999999998</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B102">
+        <v>4.4119650000000004</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B103">
+        <v>0.14935000000000001</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B104">
+        <v>1.4899999999999999E-4</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B105">
+        <v>0.154192</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B106">
+        <v>5.8381309999999997</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B107">
+        <v>3.3108900000000001</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B108">
+        <v>81515.12</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B109">
+        <v>0.81</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B110">
         <v>3478.4956000000002</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
+      <c r="C110" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B111">
+        <v>3.4784950000000001</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B112">
+        <v>3.3108900000000001</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B113">
+        <v>93.760174000000006</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B114">
+        <v>93.778442999999996</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B116">
+        <v>2.4306019999999999</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B117">
+        <v>2.4299999999999999E-3</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B118">
+        <v>2.5771790000000001</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>